<commit_message>
test[godot]: godot test unit
</commit_message>
<xml_diff>
--- a/single-boot/src/test/resources/excel/GodotCommonResource.xlsx
+++ b/single-boot/src/test/resources/excel/GodotCommonResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tank-game-server\single-boot\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2F8D26-5D90-43AF-B2C5-6DED114F1F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304575A4-60AA-4277-A8E3-775363522764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1121,7 +1121,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
@@ -1183,7 +1183,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="1">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>34</v>
@@ -1194,7 +1194,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="1">
-        <v>330</v>
+        <v>350</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>35</v>
@@ -1249,7 +1249,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="1">
-        <v>-220</v>
+        <v>-200</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>19</v>
@@ -1260,7 +1260,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="1">
-        <v>-330</v>
+        <v>-250</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
@@ -1271,7 +1271,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="1">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>27</v>
@@ -1304,7 +1304,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="1">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>25</v>

</xml_diff>